<commit_message>
add tissue source choices #47
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Sample_submission.xlsx
+++ b/fms_core/static/submission_templates/Sample_submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kseni\Documents\fms\fms_core\static\submission_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D75A9E-86DE-4B4C-8326-4202FDA6A8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B764720-D239-429F-9DCA-22798CEC8A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleSubmission" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="435">
   <si>
     <t>96-Coord</t>
   </si>
@@ -1310,6 +1310,27 @@
   </si>
   <si>
     <t>P24</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Saliva</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>Buffy coat</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>Cells</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1448,6 +1469,7 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1665,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -17498,9 +17520,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -17512,7 +17536,7 @@
     <col min="7" max="26" width="9.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17534,8 +17558,11 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H1" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -17557,8 +17584,11 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H2" s="14" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -17580,8 +17610,11 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H3" s="14" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -17600,8 +17633,11 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H4" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -17611,32 +17647,44 @@
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H5" s="14" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H6" s="14" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H7" s="14" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H8" s="14" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -17644,7 +17692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -17652,7 +17700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -17660,7 +17708,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -17668,7 +17716,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -17676,7 +17724,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -17684,7 +17732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -17692,7 +17740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>